<commit_message>
updated with two new bug
</commit_message>
<xml_diff>
--- a/demoqa.xlsx
+++ b/demoqa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\np930\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CD6827-42E2-4B5D-821F-DAB04C029C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A2256A-838F-42C5-99DB-0C73AE1C8EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65DA7BEA-066A-4FB2-86CE-CB2E0E736F51}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{65DA7BEA-066A-4FB2-86CE-CB2E0E736F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t xml:space="preserve">Test Case ID </t>
   </si>
@@ -187,6 +187,37 @@
   </si>
   <si>
     <t>checking DOB with same date of testing or even future dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	JavaScript Injection in
+ address field</t>
+  </si>
+  <si>
+    <t>Enter 
+&lt;script&gt;alert(1)&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>&lt;script&gt;alert(1)&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>Input sanitized or error shown</t>
+  </si>
+  <si>
+    <t>Form accepted (bug)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Submit form with
+ whitespace in name fields</t>
+  </si>
+  <si>
+    <t>Enter only spaces in 
+first/last name</t>
+  </si>
+  <si>
+    <t>" "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Error shown or submission blocked</t>
   </si>
 </sst>
 </file>
@@ -231,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -253,6 +284,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -276,16 +310,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>842211</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>168441</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>560997</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>59584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>72190</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>118533</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>398761</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>117929</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -300,8 +334,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1451811" y="5273841"/>
-          <a:ext cx="7671246" cy="8145825"/>
+          <a:off x="560997" y="6745227"/>
+          <a:ext cx="7666407" cy="14391202"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -738,6 +772,318 @@
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>Bug#4 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>JavaScript Injection Accepted in Address Field</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Title</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: Form accepts raw JavaScript without sanitization</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Description</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: The address field on the form allows raw HTML/JavaScript to be submitted without any validation or sanitization, indicating a potential Cross-Site Scripting (XSS) vulnerability.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Steps to Reproduce</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Fill in all required fields with valid data</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>In the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Current Address</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> field, enter: &lt;script&gt;alert(1)&lt;/script&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Click on the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Submit</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> button</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Expected Behavior</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: The form should escape or block script tags and reject malicious input with a validation error or warning.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Actual Behavior</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: The form accepts the input and submits successfully, without sanitization or any warning.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Impact</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: This opens up the possibility of </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>stored or reflected XSS attacks</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>, depending on how submitted data is later handled or displayed.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Severity</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>High</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Priority</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>High</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Bug #5 – Whitespace-Only Names Are Accepted</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Title</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: Form accepts only whitespace characters in required name fields</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Description</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: The form's validation does not prevent users from submitting first and last names that consist solely of space characters. This bypasses the purpose of the field and results in logically invalid input.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Steps to Reproduce</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Enter " " (space) in the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>First Name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> field</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Enter " " (space) in the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Last Name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> field</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Fill all other fields with valid data</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Click the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Submit</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> button</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Expected Behavior</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: The form should trim and validate the input. If the input is only whitespace, it should display an error message or block submission.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Actual Behavior</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: The form accepts the whitespace input and submits successfully.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Impact</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: This allows users to bypass required field validations, resulting in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>invalid user data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> being submitted and potentially causing issues downstream in data processing or user management systems.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Severity</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Medium</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Priority</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Medium</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -814,10 +1160,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1137,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41AB8953-09CF-4075-9B3F-486B0D836A35}">
-  <dimension ref="B3:I10"/>
+  <dimension ref="B3:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="111" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,6 +1703,58 @@
         <v>32</v>
       </c>
     </row>
+    <row r="11" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{7B08BDC4-6D43-4F08-A90A-7CD0135EE9DC}"/>

</xml_diff>